<commit_message>
update BOM with barrel jack
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="176">
   <si>
     <t>Qty</t>
   </si>
@@ -215,325 +215,331 @@
     <t>SS310A</t>
   </si>
   <si>
+    <t>J10</t>
+  </si>
+  <si>
+    <t>Conn_01x01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	CP-002AH-ND</t>
+  </si>
+  <si>
+    <t>PJ-002AH</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>Conn_01x05</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>Conn_01x04</t>
+  </si>
+  <si>
+    <t>WM4330-ND</t>
+  </si>
+  <si>
+    <t>0470531000</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>Conn_01x08</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>Conn_01x02</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>150nH</t>
+  </si>
+  <si>
+    <t>513-1568-1-ND</t>
+  </si>
+  <si>
+    <t>FP1005R1-R15-R</t>
+  </si>
+  <si>
+    <t>Q1, Q2</t>
+  </si>
+  <si>
+    <t>CSD17311Q5</t>
+  </si>
+  <si>
+    <t>296-27625-1-ND</t>
+  </si>
+  <si>
+    <t>R1, R4, R9</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>311-10KJRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-0710KL</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>5.6k</t>
+  </si>
+  <si>
+    <t>13-RC0402FR-135K6LCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-135K6L</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>3.83k</t>
+  </si>
+  <si>
+    <t>311-3.83KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-073K83L</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>100k</t>
+  </si>
+  <si>
+    <t>311-100KJRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402JR-07100KL</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>4.12k</t>
+  </si>
+  <si>
+    <t>RMCF0402FT4K12CT-ND</t>
+  </si>
+  <si>
+    <t>RMCF0402FT4K12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>1.33k</t>
+  </si>
+  <si>
+    <t>311-1.33KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-071K33L</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>4.99k</t>
+  </si>
+  <si>
+    <t>311-4.99KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-074K99L</t>
+  </si>
+  <si>
+    <t>R15</t>
+  </si>
+  <si>
+    <t>3.32k</t>
+  </si>
+  <si>
+    <t>311-3.32KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-073K32L</t>
+  </si>
+  <si>
+    <t>R16</t>
+  </si>
+  <si>
+    <t>80k</t>
+  </si>
+  <si>
+    <t>311-80.6KLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-0780K6L</t>
+  </si>
+  <si>
+    <t>SW1, SW2</t>
+  </si>
+  <si>
+    <t>GT-TC029B-H025-L1N</t>
+  </si>
+  <si>
+    <t>2449-CS1213AGF260CT-ND</t>
+  </si>
+  <si>
+    <t>CS1213AGF260</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>25MHz</t>
+  </si>
+  <si>
+    <t>1908-O250-JO32-B-1V3-1-T1-LFCT-ND</t>
+  </si>
+  <si>
+    <t>O 25,0-JO32-B-1V3-1-T1-LF</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>TXB0104RGYR</t>
+  </si>
+  <si>
+    <t>296-21930-1-ND</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>MCP1824T-1802E</t>
+  </si>
+  <si>
+    <t>MCP1824T-1802E/OTCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1824T-1802E/OT</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>MCP1824T-0802E</t>
+  </si>
+  <si>
+    <t>MCP1824T-0802E/OTCT-ND</t>
+  </si>
+  <si>
+    <t>MCP1824T-0802E/OT</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>EMC2101</t>
+  </si>
+  <si>
+    <t>EMC2101-R-ACZL-CT-ND</t>
+  </si>
+  <si>
+    <t>EMC2101-R-ACZL-TR</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>INA260</t>
+  </si>
+  <si>
+    <t>296-47777-1-ND</t>
+  </si>
+  <si>
+    <t>INA260AIPWR</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>TPS40305</t>
+  </si>
+  <si>
+    <t>296-37445-1-ND</t>
+  </si>
+  <si>
+    <t>TPS40305DRCR</t>
+  </si>
+  <si>
+    <t>U10</t>
+  </si>
+  <si>
+    <t>DS4432U+</t>
+  </si>
+  <si>
+    <t>DS4432U+-ND</t>
+  </si>
+  <si>
+    <t>U11</t>
+  </si>
+  <si>
+    <t>RT9080-33GJ5</t>
+  </si>
+  <si>
+    <t>1028-1509-1-ND</t>
+  </si>
+  <si>
+    <t>U12</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1</t>
+  </si>
+  <si>
+    <t>1965-ESP32-S3-WROOM-1-N16R8CT-ND</t>
+  </si>
+  <si>
+    <t>ESP32-S3-WROOM-1-N16R8</t>
+  </si>
+  <si>
+    <t>U14</t>
+  </si>
+  <si>
+    <t>BM1366_mode0</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>USB4105-GF-A</t>
+  </si>
+  <si>
+    <t>609-4616-1-ND</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>32.768kHz</t>
+  </si>
+  <si>
+    <t>728-1074-1-ND</t>
+  </si>
+  <si>
+    <t>SC32S-7PF20PPM</t>
+  </si>
+  <si>
     <t>J1, J2</t>
   </si>
   <si>
-    <t>Conn_01x01</t>
-  </si>
-  <si>
     <t>A100886CT-ND</t>
-  </si>
-  <si>
-    <t>63862-1</t>
-  </si>
-  <si>
-    <t>J3</t>
-  </si>
-  <si>
-    <t>Conn_01x05</t>
-  </si>
-  <si>
-    <t>J4</t>
-  </si>
-  <si>
-    <t>Conn_01x04</t>
-  </si>
-  <si>
-    <t>WM4330-ND</t>
-  </si>
-  <si>
-    <t>0470531000</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>Conn_01x08</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>L1</t>
-  </si>
-  <si>
-    <t>150nH</t>
-  </si>
-  <si>
-    <t>513-1568-1-ND</t>
-  </si>
-  <si>
-    <t>FP1005R1-R15-R</t>
-  </si>
-  <si>
-    <t>Q1, Q2</t>
-  </si>
-  <si>
-    <t>CSD17311Q5</t>
-  </si>
-  <si>
-    <t>296-27625-1-ND</t>
-  </si>
-  <si>
-    <t>R1, R4, R9</t>
-  </si>
-  <si>
-    <t>10k</t>
-  </si>
-  <si>
-    <t>311-10KJRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402JR-0710KL</t>
-  </si>
-  <si>
-    <t>R2</t>
-  </si>
-  <si>
-    <t>5.6k</t>
-  </si>
-  <si>
-    <t>13-RC0402FR-135K6LCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-135K6L</t>
-  </si>
-  <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>3.83k</t>
-  </si>
-  <si>
-    <t>311-3.83KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-073K83L</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>311-100KJRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402JR-07100KL</t>
-  </si>
-  <si>
-    <t>R12</t>
-  </si>
-  <si>
-    <t>4.12k</t>
-  </si>
-  <si>
-    <t>RMCF0402FT4K12CT-ND</t>
-  </si>
-  <si>
-    <t>RMCF0402FT4K12</t>
-  </si>
-  <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>1.33k</t>
-  </si>
-  <si>
-    <t>311-1.33KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-071K33L</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>4.99k</t>
-  </si>
-  <si>
-    <t>311-4.99KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-074K99L</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>3.32k</t>
-  </si>
-  <si>
-    <t>311-3.32KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-073K32L</t>
-  </si>
-  <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>80k</t>
-  </si>
-  <si>
-    <t>311-80.6KLRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402FR-0780K6L</t>
-  </si>
-  <si>
-    <t>SW1, SW2</t>
-  </si>
-  <si>
-    <t>GT-TC029B-H025-L1N</t>
-  </si>
-  <si>
-    <t>2449-CS1213AGF260CT-ND</t>
-  </si>
-  <si>
-    <t>CS1213AGF260</t>
-  </si>
-  <si>
-    <t>U1</t>
-  </si>
-  <si>
-    <t>25MHz</t>
-  </si>
-  <si>
-    <t>1908-O250-JO32-B-1V3-1-T1-LFCT-ND</t>
-  </si>
-  <si>
-    <t>O 25,0-JO32-B-1V3-1-T1-LF</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>TXB0104RGYR</t>
-  </si>
-  <si>
-    <t>296-21930-1-ND</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>MCP1824T-1802E</t>
-  </si>
-  <si>
-    <t>MCP1824T-1802E/OTCT-ND</t>
-  </si>
-  <si>
-    <t>MCP1824T-1802E/OT</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>MCP1824T-0802E</t>
-  </si>
-  <si>
-    <t>MCP1824T-0802E/OTCT-ND</t>
-  </si>
-  <si>
-    <t>MCP1824T-0802E/OT</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>EMC2101</t>
-  </si>
-  <si>
-    <t>EMC2101-R-ACZL-CT-ND</t>
-  </si>
-  <si>
-    <t>EMC2101-R-ACZL-TR</t>
-  </si>
-  <si>
-    <t>U8</t>
-  </si>
-  <si>
-    <t>INA260</t>
-  </si>
-  <si>
-    <t>296-47777-1-ND</t>
-  </si>
-  <si>
-    <t>INA260AIPWR</t>
-  </si>
-  <si>
-    <t>U9</t>
-  </si>
-  <si>
-    <t>TPS40305</t>
-  </si>
-  <si>
-    <t>296-37445-1-ND</t>
-  </si>
-  <si>
-    <t>TPS40305DRCR</t>
-  </si>
-  <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>DS4432U+</t>
-  </si>
-  <si>
-    <t>DS4432U+-ND</t>
-  </si>
-  <si>
-    <t>U11</t>
-  </si>
-  <si>
-    <t>RT9080-33GJ5</t>
-  </si>
-  <si>
-    <t>1028-1509-1-ND</t>
-  </si>
-  <si>
-    <t>U12</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1</t>
-  </si>
-  <si>
-    <t>1965-ESP32-S3-WROOM-1-N16R8CT-ND</t>
-  </si>
-  <si>
-    <t>ESP32-S3-WROOM-1-N16R8</t>
-  </si>
-  <si>
-    <t>U14</t>
-  </si>
-  <si>
-    <t>BM1366_mode0</t>
-  </si>
-  <si>
-    <t>J8</t>
-  </si>
-  <si>
-    <t>USB4105-GF-A</t>
-  </si>
-  <si>
-    <t>609-4616-1-ND</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>32.768kHz</t>
-  </si>
-  <si>
-    <t>728-1074-1-ND</t>
-  </si>
-  <si>
-    <t>SC32S-7PF20PPM</t>
   </si>
 </sst>
 </file>
@@ -556,7 +562,6 @@
     <font>
       <color theme="1"/>
       <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -817,7 +822,6 @@
     <col customWidth="1" min="1" max="1" width="5.71"/>
     <col customWidth="1" min="2" max="5" width="30.71"/>
     <col customWidth="1" min="6" max="6" width="5.71"/>
-    <col customWidth="1" min="7" max="26" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1116,16 +1120,16 @@
       <c r="A18" s="2">
         <v>2.0</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1570,16 +1574,16 @@
       <c r="A48" s="2">
         <v>1.0</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="3" t="s">
+      <c r="C48" s="2" t="s">
         <v>168</v>
       </c>
       <c r="D48" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="E48" s="2" t="s">
         <v>168</v>
       </c>
     </row>
@@ -2571,7 +2575,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="5.71"/>
     <col customWidth="1" min="2" max="4" width="30.71"/>
-    <col customWidth="1" min="5" max="26" width="8.86"/>
+    <col customWidth="1" min="5" max="6" width="8.86"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2766,10 +2770,10 @@
         <v>2.0</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>67</v>
+        <v>174</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>69</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19">
@@ -3029,10 +3033,10 @@
       <c r="A42" s="2">
         <v>1.0</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added display power, gerbers, bom
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
   <si>
     <t>Qty</t>
   </si>
@@ -215,16 +215,13 @@
     <t>SS310A</t>
   </si>
   <si>
-    <t>J10</t>
-  </si>
-  <si>
-    <t>Conn_01x01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        CP-002AH-ND</t>
-  </si>
-  <si>
-    <t>PJ-002AH</t>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>PJ-037AH</t>
+  </si>
+  <si>
+    <t>CP-037AH-ND</t>
   </si>
   <si>
     <t>J3</t>
@@ -536,14 +533,20 @@
     <t>SC32S-7PF20PPM</t>
   </si>
   <si>
-    <t>CP-002AH-ND</t>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>455-B2B-XH-A-ND</t>
+  </si>
+  <si>
+    <t>B2B-XH-A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -561,8 +564,14 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-      <name val="Docs-Calibri"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9.0"/>
+      <color rgb="FF444444"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="4">
@@ -597,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -606,7 +615,14 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -1127,20 +1143,20 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>1.0</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D18" s="4" t="s">
         <v>69</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19">
@@ -1148,10 +1164,10 @@
         <v>1.0</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="20">
@@ -1159,16 +1175,16 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="D20" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -1176,10 +1192,10 @@
         <v>1.0</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -1187,10 +1203,10 @@
         <v>1.0</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -1198,16 +1214,16 @@
         <v>1.0</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -1215,16 +1231,16 @@
         <v>2.0</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>87</v>
-      </c>
       <c r="E24" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -1232,16 +1248,16 @@
         <v>3.0</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D25" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -1249,16 +1265,16 @@
         <v>1.0</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1"/>
@@ -1267,16 +1283,16 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="E28" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -1284,16 +1300,16 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1301,16 +1317,16 @@
         <v>1.0</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="E30" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1318,16 +1334,16 @@
         <v>1.0</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="D31" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="E31" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -1335,16 +1351,16 @@
         <v>1.0</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -1352,16 +1368,16 @@
         <v>1.0</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="D33" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -1369,16 +1385,16 @@
         <v>1.0</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1"/>
@@ -1387,16 +1403,16 @@
         <v>2.0</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -1404,16 +1420,16 @@
         <v>1.0</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -1421,16 +1437,16 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="2" t="s">
+      <c r="D38" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -1438,16 +1454,16 @@
         <v>1.0</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -1455,16 +1471,16 @@
         <v>1.0</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="E40" s="2" t="s">
         <v>141</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -1472,16 +1488,16 @@
         <v>1.0</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -1489,16 +1505,16 @@
         <v>1.0</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>149</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -1506,16 +1522,16 @@
         <v>1.0</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -1523,16 +1539,16 @@
         <v>1.0</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C44" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="D44" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>157</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -1540,16 +1556,16 @@
         <v>1.0</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -1557,16 +1573,16 @@
         <v>1.0</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C46" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -1574,10 +1590,10 @@
         <v>1.0</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C47" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -1585,16 +1601,16 @@
         <v>1.0</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="E48" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -1602,19 +1618,35 @@
         <v>1.0</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="E49" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="E49" s="2" t="s">
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="B50" s="5" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1"/>
+      <c r="C50" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
     <row r="51" ht="15.75" customHeight="1"/>
     <row r="52" ht="15.75" customHeight="1"/>
     <row r="53" ht="15.75" customHeight="1"/>
@@ -2776,14 +2808,14 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3">
+      <c r="A18" s="2">
         <v>1.0</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>174</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19">
@@ -2791,10 +2823,10 @@
         <v>1.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="20">
@@ -2802,10 +2834,10 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -2813,10 +2845,10 @@
         <v>2.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -2824,10 +2856,10 @@
         <v>3.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -2835,10 +2867,10 @@
         <v>1.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -2846,10 +2878,10 @@
         <v>1.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -2857,10 +2889,10 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2868,10 +2900,10 @@
         <v>1.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -2879,10 +2911,10 @@
         <v>1.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -2890,10 +2922,10 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -2901,10 +2933,10 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -2912,10 +2944,10 @@
         <v>1.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -2923,10 +2955,10 @@
         <v>2.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -2934,10 +2966,10 @@
         <v>1.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -2945,10 +2977,10 @@
         <v>1.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -2956,10 +2988,10 @@
         <v>1.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -2967,10 +2999,10 @@
         <v>1.0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -2978,10 +3010,10 @@
         <v>1.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -2989,10 +3021,10 @@
         <v>1.0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -3000,10 +3032,10 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -3011,10 +3043,10 @@
         <v>1.0</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -3022,10 +3054,10 @@
         <v>1.0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -3033,10 +3065,10 @@
         <v>1.0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -3044,10 +3076,10 @@
         <v>1.0</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -3055,13 +3087,23 @@
         <v>1.0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="44" ht="15.75" customHeight="1"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="44" ht="15.75" customHeight="1">
+      <c r="A44" s="5">
+        <v>2.0</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>174</v>
+      </c>
+    </row>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>
     <row r="47" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
fix JSX, updated boms
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="179">
   <si>
     <t>Qty</t>
   </si>
@@ -209,10 +209,10 @@
     <t>SS310</t>
   </si>
   <si>
-    <t>3191-SS310ACT-ND</t>
-  </si>
-  <si>
-    <t>SS310A</t>
+    <t>SK310A-LTPMSCT-ND</t>
+  </si>
+  <si>
+    <t>SK310A-LTP</t>
   </si>
   <si>
     <t>J1</t>
@@ -224,6 +224,12 @@
     <t>CP-037AH-ND</t>
   </si>
   <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>if J1 used</t>
+  </si>
+  <si>
     <t>J3</t>
   </si>
   <si>
@@ -242,9 +248,6 @@
     <t>0470531000</t>
   </si>
   <si>
-    <t>J6</t>
-  </si>
-  <si>
     <t>Conn_01x08</t>
   </si>
   <si>
@@ -540,13 +543,19 @@
   </si>
   <si>
     <t>B2B-XH-A</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>J10</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -568,13 +577,8 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9.0"/>
-      <color rgb="FF444444"/>
-      <name val="Roboto"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -585,12 +589,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFA0A0A0"/>
         <bgColor rgb="FFA0A0A0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -606,7 +604,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -618,12 +616,6 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1135,10 +1127,10 @@
       <c r="C17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1160,13 +1152,22 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="A19" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>71</v>
       </c>
     </row>
@@ -1180,21 +1181,21 @@
       <c r="C20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E20" s="2" t="s">
-        <v>75</v>
-      </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="2">
         <v>1.0</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>77</v>
       </c>
     </row>
@@ -1203,10 +1204,10 @@
         <v>1.0</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -1214,102 +1215,96 @@
         <v>1.0</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="2">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="E25" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="2">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C26" s="2" t="s">
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="2">
-        <v>1.0</v>
-      </c>
-      <c r="B28" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
+    </row>
+    <row r="28" ht="15.75" customHeight="1"/>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="2">
         <v>1.0</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="E29" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -1317,16 +1312,16 @@
         <v>1.0</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -1334,16 +1329,16 @@
         <v>1.0</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -1351,16 +1346,16 @@
         <v>1.0</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -1368,16 +1363,16 @@
         <v>1.0</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E33" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -1385,51 +1380,51 @@
         <v>1.0</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C34" s="2" t="s">
+    </row>
+    <row r="35" ht="15.75" customHeight="1">
+      <c r="A35" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B35" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="C35" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="35" ht="15.75" customHeight="1"/>
-    <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="2">
-        <v>2.0</v>
-      </c>
-      <c r="B36" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
+    </row>
+    <row r="36" ht="15.75" customHeight="1"/>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="2">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E37" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -1437,16 +1432,16 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -1454,16 +1449,16 @@
         <v>1.0</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>136</v>
-      </c>
       <c r="E39" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -1471,16 +1466,16 @@
         <v>1.0</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>138</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -1488,16 +1483,16 @@
         <v>1.0</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -1505,16 +1500,16 @@
         <v>1.0</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>146</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -1522,16 +1517,16 @@
         <v>1.0</v>
       </c>
       <c r="B43" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -1539,16 +1534,16 @@
         <v>1.0</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E44" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -1556,16 +1551,16 @@
         <v>1.0</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C45" s="2" t="s">
-        <v>158</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="E45" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
@@ -1573,16 +1568,16 @@
         <v>1.0</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>162</v>
-      </c>
       <c r="E46" s="2" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -1590,10 +1585,16 @@
         <v>1.0</v>
       </c>
       <c r="B47" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E47" s="2" t="s">
         <v>164</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -1601,16 +1602,10 @@
         <v>1.0</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C48" s="2" t="s">
         <v>166</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1">
@@ -1618,37 +1613,75 @@
         <v>1.0</v>
       </c>
       <c r="B49" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="E49" s="2" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="50" ht="15.75" customHeight="1">
+      <c r="A50" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="B50" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="B50" s="5" t="s">
+      <c r="E50" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="6" t="s">
+    </row>
+    <row r="51" ht="15.75" customHeight="1">
+      <c r="A51" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>174</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="C51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D51" s="4" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="51" ht="15.75" customHeight="1"/>
-    <row r="52" ht="15.75" customHeight="1"/>
+      <c r="E51" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="52" ht="15.75" customHeight="1">
+      <c r="A52" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>177</v>
+      </c>
+    </row>
     <row r="53" ht="15.75" customHeight="1"/>
     <row r="54" ht="15.75" customHeight="1"/>
     <row r="55" ht="15.75" customHeight="1"/>
@@ -2803,7 +2836,7 @@
       <c r="B17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -2823,10 +2856,10 @@
         <v>1.0</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20">
@@ -2834,10 +2867,10 @@
         <v>1.0</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1">
@@ -2845,10 +2878,10 @@
         <v>2.0</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1">
@@ -2856,10 +2889,10 @@
         <v>3.0</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
@@ -2867,10 +2900,10 @@
         <v>1.0</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1">
@@ -2878,10 +2911,10 @@
         <v>1.0</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1">
@@ -2889,10 +2922,10 @@
         <v>1.0</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1">
@@ -2900,10 +2933,10 @@
         <v>1.0</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1">
@@ -2911,10 +2944,10 @@
         <v>1.0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1">
@@ -2922,10 +2955,10 @@
         <v>1.0</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
@@ -2933,10 +2966,10 @@
         <v>1.0</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
@@ -2944,10 +2977,10 @@
         <v>1.0</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1">
@@ -2955,10 +2988,10 @@
         <v>2.0</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
@@ -2966,10 +2999,10 @@
         <v>1.0</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1">
@@ -2977,10 +3010,10 @@
         <v>1.0</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1">
@@ -2988,10 +3021,10 @@
         <v>1.0</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
@@ -2999,10 +3032,10 @@
         <v>1.0</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
@@ -3010,10 +3043,10 @@
         <v>1.0</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
@@ -3021,10 +3054,10 @@
         <v>1.0</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
@@ -3032,10 +3065,10 @@
         <v>1.0</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
@@ -3043,10 +3076,10 @@
         <v>1.0</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -3054,10 +3087,10 @@
         <v>1.0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -3065,10 +3098,10 @@
         <v>1.0</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -3076,10 +3109,10 @@
         <v>1.0</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -3087,21 +3120,21 @@
         <v>1.0</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="5">
-        <v>2.0</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="C44" s="6" t="s">
+      <c r="A44" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="B44" s="4" t="s">
         <v>174</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
added PWR_EN signal to shutdown the TPS40305
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10314"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra-v1.1/Manufacturing Files/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9B15BE-06A8-9F4A-9495-F4F61D993D83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="25280" windowHeight="22700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="DK Order" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="179">
   <si>
     <t>Qty</t>
   </si>
@@ -35,6 +29,9 @@
     <t>DK</t>
   </si>
   <si>
+    <t>Manufacturer</t>
+  </si>
+  <si>
     <t>PARTNO</t>
   </si>
   <si>
@@ -212,6 +209,9 @@
     <t>SK310A-LTPMSCT-ND</t>
   </si>
   <si>
+    <t>迪一</t>
+  </si>
+  <si>
     <t>SK310A-LTP</t>
   </si>
   <si>
@@ -279,6 +279,18 @@
   </si>
   <si>
     <t>296-27625-1-ND</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>2N7002K</t>
+  </si>
+  <si>
+    <t>2N7002KWCT-ND</t>
+  </si>
+  <si>
+    <t>2N7002KW</t>
   </si>
   <si>
     <t>R1, R4, R6, R9</t>
@@ -545,8 +557,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -598,14 +610,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -652,7 +656,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -684,27 +688,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -736,24 +722,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -929,21 +897,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="6" width="30.7109375" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -962,747 +928,770 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D12" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="F16" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D17" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" t="s">
-        <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+      <c r="F18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D21" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="F21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="F22" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F23" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+      <c r="F24" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>97</v>
+      </c>
+      <c r="D25" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1</v>
-      </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="F26" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="F27" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="F28" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="F29" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+      <c r="F30" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+      <c r="F31" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+      <c r="F32" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" t="s">
+        <v>130</v>
+      </c>
+      <c r="F33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1</v>
-      </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+      <c r="F34" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D35" t="s">
-        <v>136</v>
-      </c>
-      <c r="E35" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+      <c r="F35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C36" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D36" t="s">
-        <v>139</v>
-      </c>
-      <c r="E36" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+      <c r="F36" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="F37" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="F38" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+      <c r="F39" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+      <c r="F40" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D41" t="s">
-        <v>159</v>
-      </c>
-      <c r="E41" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+      <c r="F41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="D42" t="s">
-        <v>162</v>
-      </c>
-      <c r="E42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+      <c r="F42" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="D43" t="s">
-        <v>165</v>
-      </c>
-      <c r="E43" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="F43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="D44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
-      </c>
-      <c r="D45" t="s">
-        <v>171</v>
-      </c>
-      <c r="E45" t="s">
-        <v>172</v>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" t="s">
+        <v>176</v>
+      </c>
+      <c r="D46" t="s">
+        <v>177</v>
+      </c>
+      <c r="F46" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -1711,20 +1700,18 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C44"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.6640625" customWidth="1"/>
-    <col min="2" max="4" width="30.6640625" customWidth="1"/>
+    <col min="1" max="1" width="5.7109375" customWidth="1"/>
+    <col min="2" max="4" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1735,469 +1722,469 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
         <v>4</v>
       </c>
-      <c r="B23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
       <c r="B24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
       <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
         <v>2</v>
       </c>
-      <c r="B25" t="s">
-        <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>1</v>
-      </c>
       <c r="B26" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C31" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C32" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
       <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>128</v>
+      </c>
+      <c r="C33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
         <v>2</v>
       </c>
-      <c r="B33" t="s">
-        <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1</v>
-      </c>
       <c r="B34" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C34" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C35" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C36" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="C38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C41" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2206,6 +2193,25 @@
       </c>
       <c r="C44" t="s">
         <v>171</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" t="s">
+        <v>177</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- added fix for #96 and #97 - beefed up vias for new SMD barrel connector - added PWR_EN pullup - added PLUG_SENSE signal to GPIO12 - Regenerated BOM - Added gerbers - Added missing 3D files
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="183">
   <si>
     <t>Qty</t>
   </si>
@@ -38,7 +38,7 @@
     <t>DNP</t>
   </si>
   <si>
-    <t>C1, C7, C9, C19, C20, C22, C23, C29, C33, C42, C52</t>
+    <t>C1, C7, C9, C19, C20, C29, C33, C42, C52</t>
   </si>
   <si>
     <t>0.1uF</t>
@@ -50,7 +50,7 @@
     <t>0402X104K100CT</t>
   </si>
   <si>
-    <t>C2, C3, C4, C5, C6, C8, C10, C11, C12, C14, C15, C16, C17, C18, C21, C24, C25, C27, C35, C44, C49</t>
+    <t>C2, C3, C4, C5, C6, C8, C10, C11, C12, C14, C15, C16, C17, C18, C21, C22, C23, C24, C25, C27, C35, C44, C49</t>
   </si>
   <si>
     <t>1uF</t>
@@ -218,10 +218,10 @@
     <t>J1</t>
   </si>
   <si>
-    <t>PJ-037AH</t>
-  </si>
-  <si>
-    <t>CP-037AH-ND</t>
+    <t>54-00164</t>
+  </si>
+  <si>
+    <t>839-54-00164CT-ND</t>
   </si>
   <si>
     <t>J2</t>
@@ -293,7 +293,7 @@
     <t>2N7002KW</t>
   </si>
   <si>
-    <t>R1, R4, R6, R9</t>
+    <t>R1, R4, R6, R7, R9</t>
   </si>
   <si>
     <t>10k</t>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>RMCF0402JT5K10</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>1M</t>
+  </si>
+  <si>
+    <t>311-1.00MLRCT-ND</t>
+  </si>
+  <si>
+    <t>RC0402FR-071ML</t>
   </si>
   <si>
     <t>R10</t>
@@ -898,7 +910,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -934,7 +946,7 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -951,7 +963,7 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1190,7 +1202,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1207,7 +1219,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1224,7 +1236,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1241,7 +1253,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1258,7 +1270,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1275,7 +1287,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1292,7 +1304,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1309,9 +1321,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:7">
       <c r="A24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>92</v>
@@ -1326,7 +1338,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1343,7 +1355,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:7">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1360,7 +1372,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:7">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1377,7 +1389,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:7">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1394,7 +1406,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:7">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1410,8 +1422,11 @@
       <c r="F29" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1428,7 +1443,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:7">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1445,7 +1460,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:7">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1481,7 +1496,7 @@
     </row>
     <row r="34" spans="1:6">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
         <v>132</v>
@@ -1498,7 +1513,7 @@
     </row>
     <row r="35" spans="1:6">
       <c r="A35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B35" t="s">
         <v>136</v>
@@ -1527,7 +1542,7 @@
         <v>142</v>
       </c>
       <c r="F36" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1535,16 +1550,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="C37" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="D37" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" t="s">
         <v>145</v>
-      </c>
-      <c r="F37" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1629,7 +1644,7 @@
         <v>165</v>
       </c>
       <c r="F42" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1637,16 +1652,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C43" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D43" t="s">
+        <v>169</v>
+      </c>
+      <c r="F43" t="s">
         <v>168</v>
-      </c>
-      <c r="F43" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1654,16 +1669,16 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D44" t="s">
+        <v>172</v>
+      </c>
+      <c r="F44" t="s">
         <v>171</v>
-      </c>
-      <c r="F44" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1676,22 +1691,39 @@
       <c r="C45" t="s">
         <v>174</v>
       </c>
+      <c r="D45" t="s">
+        <v>175</v>
+      </c>
+      <c r="F45" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="46" spans="1:6">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>176</v>
-      </c>
-      <c r="D46" t="s">
-        <v>177</v>
-      </c>
-      <c r="F46" t="s">
         <v>178</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>179</v>
+      </c>
+      <c r="C47" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" t="s">
+        <v>181</v>
+      </c>
+      <c r="F47" t="s">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -1724,7 +1756,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1735,7 +1767,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -1966,7 +1998,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>92</v>
@@ -2024,10 +2056,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C29" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2035,10 +2067,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C30" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2046,10 +2078,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2057,10 +2089,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="C32" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2068,10 +2100,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C33" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2079,10 +2111,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C34" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2090,10 +2122,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2101,10 +2133,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="C36" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2112,10 +2144,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2123,10 +2155,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="C38" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2134,10 +2166,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C39" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2145,10 +2177,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="C40" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2156,10 +2188,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="C41" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2167,10 +2199,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="C42" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2178,10 +2210,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="C43" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2189,10 +2221,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2200,7 +2232,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2208,10 +2240,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C46" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated BOM xlsx and added Gerbers
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra-v1.1/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CB532DA-701D-3E4C-826C-954FA6D90D8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4E68F2-4458-B748-ACB0-55310C98B91E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="31580" windowHeight="25320" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="33760" windowHeight="25840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="177">
   <si>
     <t>Qty</t>
   </si>
@@ -351,18 +351,6 @@
   </si>
   <si>
     <t>RC0402FR-073K83L</t>
-  </si>
-  <si>
-    <t>R11</t>
-  </si>
-  <si>
-    <t>100k</t>
-  </si>
-  <si>
-    <t>311-100KJRCT-ND</t>
-  </si>
-  <si>
-    <t>RC0402JR-07100KL</t>
   </si>
   <si>
     <t>R12</t>
@@ -954,10 +942,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N48" sqref="N48"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1242,7 +1230,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1259,7 +1247,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1276,7 +1264,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1293,7 +1281,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1310,7 +1298,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1327,7 +1315,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1344,7 +1332,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1361,7 +1349,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>5</v>
       </c>
@@ -1378,7 +1366,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1395,7 +1383,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1412,7 +1400,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -1429,7 +1417,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -1446,7 +1434,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -1462,11 +1450,8 @@
       <c r="E29" t="s">
         <v>113</v>
       </c>
-      <c r="F29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -1483,7 +1468,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -1500,7 +1485,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -1536,7 +1521,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B34" t="s">
         <v>130</v>
@@ -1553,7 +1538,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B35" t="s">
         <v>134</v>
@@ -1582,7 +1567,7 @@
         <v>140</v>
       </c>
       <c r="E36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1590,16 +1575,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" t="s">
         <v>142</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>143</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>144</v>
-      </c>
-      <c r="E37" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1684,7 +1669,7 @@
         <v>163</v>
       </c>
       <c r="E42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1692,16 +1677,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>164</v>
+      </c>
+      <c r="C43" t="s">
         <v>165</v>
       </c>
-      <c r="C43" t="s">
+      <c r="D43" t="s">
         <v>166</v>
       </c>
-      <c r="D43" t="s">
-        <v>167</v>
-      </c>
       <c r="E43" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1709,16 +1694,16 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
+        <v>167</v>
+      </c>
+      <c r="C44" t="s">
         <v>168</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>169</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>170</v>
-      </c>
-      <c r="E44" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1731,39 +1716,22 @@
       <c r="C45" t="s">
         <v>172</v>
       </c>
-      <c r="D45" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" t="s">
-        <v>174</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" t="s">
+        <v>173</v>
+      </c>
+      <c r="C46" t="s">
+        <v>174</v>
+      </c>
+      <c r="D46" t="s">
         <v>175</v>
       </c>
-      <c r="C46" t="s">
+      <c r="E46" t="s">
         <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C47" t="s">
-        <v>178</v>
-      </c>
-      <c r="D47" t="s">
-        <v>179</v>
-      </c>
-      <c r="E47" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>
@@ -2096,10 +2064,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2107,10 +2075,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C30" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2118,10 +2086,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C31" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2129,10 +2097,10 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -2140,10 +2108,10 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -2151,10 +2119,10 @@
         <v>2</v>
       </c>
       <c r="B34" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2162,10 +2130,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2173,10 +2141,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C36" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2184,10 +2152,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="C37" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2195,10 +2163,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C38" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2206,10 +2174,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2217,10 +2185,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C40" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2228,10 +2196,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2239,10 +2207,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C42" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2250,10 +2218,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C43" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2261,10 +2229,10 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -2272,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -2280,10 +2248,10 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="C46" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update J9 part number and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra-v1.1/Manufacturing Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4E68F2-4458-B748-ACB0-55310C98B91E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E1BBE-202C-3544-BD2A-66A15896674A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33760" windowHeight="25840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="33760" windowHeight="25840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="180">
   <si>
     <t>Qty</t>
   </si>
@@ -552,6 +552,15 @@
   </si>
   <si>
     <t>SC32S-7PF20PPM</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>S5596-ND</t>
+  </si>
+  <si>
+    <t>NPTC041KFXC-RC</t>
   </si>
 </sst>
 </file>
@@ -942,10 +951,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I38" sqref="I38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E58" sqref="E58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1734,6 +1743,23 @@
         <v>176</v>
       </c>
     </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+      <c r="D47" t="s">
+        <v>178</v>
+      </c>
+      <c r="E47" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1741,9 +1767,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2254,6 +2282,17 @@
         <v>175</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
+        <v>177</v>
+      </c>
+      <c r="C47" t="s">
+        <v>178</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added gerbers and BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxeUltra/Manufacturing Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxe-205/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{117E1BBE-202C-3544-BD2A-66A15896674A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2B2FE-58A6-8D4F-9695-61E1868ABFF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="33760" windowHeight="25840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="28320" windowHeight="25240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="172">
   <si>
     <t>Qty</t>
   </si>
@@ -38,9 +38,6 @@
     <t>PARTNO</t>
   </si>
   <si>
-    <t>DNP</t>
-  </si>
-  <si>
     <t>C1, C7, C9, C19, C20, C29, C33, C42, C52</t>
   </si>
   <si>
@@ -203,37 +200,13 @@
     <t>C3216X5R0J107M160AB</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
-    <t>SS310</t>
-  </si>
-  <si>
-    <t>SK310A-LTPMSCT-ND</t>
-  </si>
-  <si>
-    <t>SK310A-LTP</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
-    <t>54-00164</t>
-  </si>
-  <si>
-    <t>839-54-00164CT-ND</t>
-  </si>
-  <si>
-    <t>J2</t>
-  </si>
-  <si>
-    <t>Conn_01x02</t>
-  </si>
-  <si>
-    <t>455-B2B-XH-A-ND</t>
-  </si>
-  <si>
-    <t>B2B-XH-A</t>
+    <t>PJ-036AH-SMT</t>
+  </si>
+  <si>
+    <t>CP-036AHPJTR-ND</t>
   </si>
   <si>
     <t>J4</t>
@@ -260,6 +233,15 @@
     <t>USB4105-GF-A</t>
   </si>
   <si>
+    <t>J9</t>
+  </si>
+  <si>
+    <t>S5596-ND</t>
+  </si>
+  <si>
+    <t>NPTC041KFXC-RC</t>
+  </si>
+  <si>
     <t>L1</t>
   </si>
   <si>
@@ -554,13 +536,7 @@
     <t>SC32S-7PF20PPM</t>
   </si>
   <si>
-    <t>J9</t>
-  </si>
-  <si>
-    <t>S5596-ND</t>
-  </si>
-  <si>
-    <t>NPTC041KFXC-RC</t>
+    <t>NOPE</t>
   </si>
 </sst>
 </file>
@@ -951,20 +927,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="5" width="30.6640625" customWidth="1"/>
-    <col min="6" max="6" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -980,263 +955,260 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>23</v>
       </c>
       <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>19</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>20</v>
       </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
         <v>22</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>24</v>
       </c>
-      <c r="E6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>31</v>
       </c>
-      <c r="E8" t="s">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>1</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>33</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>35</v>
       </c>
-      <c r="E9" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>38</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>42</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
         <v>45</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>47</v>
       </c>
-      <c r="E12" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>1</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>49</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>50</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>51</v>
       </c>
-      <c r="E13" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>1</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>56</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>57</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" t="s">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>60</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>61</v>
       </c>
-      <c r="D16" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1244,13 +1216,13 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D17" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" t="s">
-        <v>66</v>
       </c>
       <c r="E17" t="s">
         <v>65</v>
@@ -1261,16 +1233,16 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
         <v>67</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1278,16 +1250,16 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="C19" t="s">
+      <c r="E19" t="s">
         <v>72</v>
-      </c>
-      <c r="D19" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1295,118 +1267,118 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
+        <v>74</v>
+      </c>
+      <c r="D20" t="s">
         <v>75</v>
       </c>
-      <c r="C20" t="s">
+      <c r="E20" t="s">
         <v>76</v>
-      </c>
-      <c r="D20" t="s">
-        <v>77</v>
-      </c>
-      <c r="E20" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
+        <v>78</v>
+      </c>
+      <c r="D21" t="s">
         <v>79</v>
       </c>
-      <c r="C21" t="s">
-        <v>80</v>
-      </c>
-      <c r="D21" t="s">
-        <v>81</v>
-      </c>
       <c r="E21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>80</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
         <v>83</v>
-      </c>
-      <c r="C22" t="s">
-        <v>84</v>
-      </c>
-      <c r="D22" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" t="s">
         <v>86</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E23" t="s">
         <v>87</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-      <c r="E23" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
         <v>90</v>
       </c>
-      <c r="C24" t="s">
+      <c r="E24" t="s">
         <v>91</v>
-      </c>
-      <c r="D24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E24" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D25" t="s">
         <v>94</v>
       </c>
-      <c r="C25" t="s">
+      <c r="E25" t="s">
         <v>95</v>
-      </c>
-      <c r="D25" t="s">
-        <v>96</v>
-      </c>
-      <c r="E25" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" t="s">
         <v>98</v>
       </c>
-      <c r="C26" t="s">
+      <c r="E26" t="s">
         <v>99</v>
-      </c>
-      <c r="D26" t="s">
-        <v>100</v>
-      </c>
-      <c r="E26" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1414,16 +1386,16 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" t="s">
         <v>102</v>
       </c>
-      <c r="C27" t="s">
+      <c r="E27" t="s">
         <v>103</v>
-      </c>
-      <c r="D27" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1431,16 +1403,16 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
+        <v>105</v>
+      </c>
+      <c r="D28" t="s">
         <v>106</v>
       </c>
-      <c r="C28" t="s">
+      <c r="E28" t="s">
         <v>107</v>
-      </c>
-      <c r="D28" t="s">
-        <v>108</v>
-      </c>
-      <c r="E28" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1448,16 +1420,16 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" t="s">
         <v>110</v>
       </c>
-      <c r="C29" t="s">
+      <c r="E29" t="s">
         <v>111</v>
-      </c>
-      <c r="D29" t="s">
-        <v>112</v>
-      </c>
-      <c r="E29" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1465,16 +1437,16 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="D30" t="s">
         <v>114</v>
       </c>
-      <c r="C30" t="s">
+      <c r="E30" t="s">
         <v>115</v>
-      </c>
-      <c r="D30" t="s">
-        <v>116</v>
-      </c>
-      <c r="E30" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -1482,16 +1454,16 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" t="s">
         <v>118</v>
       </c>
-      <c r="C31" t="s">
+      <c r="E31" t="s">
         <v>119</v>
-      </c>
-      <c r="D31" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1499,50 +1471,50 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
+        <v>121</v>
+      </c>
+      <c r="D32" t="s">
         <v>122</v>
       </c>
-      <c r="C32" t="s">
+      <c r="E32" t="s">
         <v>123</v>
-      </c>
-      <c r="D32" t="s">
-        <v>124</v>
-      </c>
-      <c r="E32" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
+        <v>125</v>
+      </c>
+      <c r="D33" t="s">
         <v>126</v>
       </c>
-      <c r="C33" t="s">
+      <c r="E33" t="s">
         <v>127</v>
-      </c>
-      <c r="D33" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
+        <v>129</v>
+      </c>
+      <c r="D34" t="s">
         <v>130</v>
       </c>
-      <c r="C34" t="s">
+      <c r="E34" t="s">
         <v>131</v>
-      </c>
-      <c r="D34" t="s">
-        <v>132</v>
-      </c>
-      <c r="E34" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1550,16 +1522,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" t="s">
         <v>134</v>
       </c>
-      <c r="C35" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" t="s">
-        <v>136</v>
-      </c>
       <c r="E35" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1567,16 +1539,16 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
+        <v>135</v>
+      </c>
+      <c r="C36" t="s">
+        <v>136</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" t="s">
         <v>138</v>
-      </c>
-      <c r="C36" t="s">
-        <v>139</v>
-      </c>
-      <c r="D36" t="s">
-        <v>140</v>
-      </c>
-      <c r="E36" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1584,16 +1556,16 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
+        <v>140</v>
+      </c>
+      <c r="D37" t="s">
         <v>141</v>
       </c>
-      <c r="C37" t="s">
+      <c r="E37" t="s">
         <v>142</v>
-      </c>
-      <c r="D37" t="s">
-        <v>143</v>
-      </c>
-      <c r="E37" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1601,16 +1573,16 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D38" t="s">
         <v>145</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>146</v>
-      </c>
-      <c r="D38" t="s">
-        <v>147</v>
-      </c>
-      <c r="E38" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1618,16 +1590,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
+        <v>148</v>
+      </c>
+      <c r="D39" t="s">
         <v>149</v>
       </c>
-      <c r="C39" t="s">
+      <c r="E39" t="s">
         <v>150</v>
-      </c>
-      <c r="D39" t="s">
-        <v>151</v>
-      </c>
-      <c r="E39" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1635,16 +1607,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
+        <v>152</v>
+      </c>
+      <c r="D40" t="s">
         <v>153</v>
       </c>
-      <c r="C40" t="s">
+      <c r="E40" t="s">
         <v>154</v>
-      </c>
-      <c r="D40" t="s">
-        <v>155</v>
-      </c>
-      <c r="E40" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1652,16 +1624,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
+        <v>156</v>
+      </c>
+      <c r="D41" t="s">
         <v>157</v>
       </c>
-      <c r="C41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D41" t="s">
-        <v>159</v>
-      </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1669,16 +1641,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1686,16 +1658,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C43" t="s">
+        <v>162</v>
+      </c>
+      <c r="D43" t="s">
+        <v>163</v>
+      </c>
+      <c r="E43" t="s">
         <v>164</v>
-      </c>
-      <c r="C43" t="s">
-        <v>165</v>
-      </c>
-      <c r="D43" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1703,16 +1675,13 @@
         <v>1</v>
       </c>
       <c r="B44" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C44" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D44" t="s">
-        <v>169</v>
-      </c>
-      <c r="E44" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1720,44 +1689,16 @@
         <v>1</v>
       </c>
       <c r="B45" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C45" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" t="s">
-        <v>174</v>
-      </c>
-      <c r="D46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E46" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
-      <c r="D47" t="s">
-        <v>178</v>
-      </c>
-      <c r="E47" t="s">
-        <v>179</v>
+        <v>168</v>
+      </c>
+      <c r="D45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E45" t="s">
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1767,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C55" sqref="C55"/>
+      <selection activeCell="D53" sqref="D53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1795,10 +1736,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1806,10 +1747,10 @@
         <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1817,10 +1758,10 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1828,10 +1769,10 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1839,10 +1780,10 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1850,10 +1791,10 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1861,10 +1802,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
         <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1872,10 +1813,10 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1883,10 +1824,10 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1894,10 +1835,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1905,10 +1846,10 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1916,10 +1857,10 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1927,10 +1868,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
         <v>53</v>
-      </c>
-      <c r="C14" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1938,10 +1879,10 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1949,10 +1890,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1960,10 +1901,10 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" t="s">
         <v>64</v>
-      </c>
-      <c r="C17" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1971,10 +1912,10 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1982,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C19" t="s">
         <v>71</v>
-      </c>
-      <c r="C19" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1993,76 +1934,76 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>73</v>
+      </c>
+      <c r="C20" t="s">
         <v>75</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
         <v>79</v>
-      </c>
-      <c r="C21" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B23" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
         <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B24" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24" t="s">
         <v>90</v>
-      </c>
-      <c r="C24" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C25" t="s">
         <v>94</v>
-      </c>
-      <c r="C25" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26" t="s">
+        <v>96</v>
+      </c>
+      <c r="C26" t="s">
         <v>98</v>
-      </c>
-      <c r="C26" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2070,10 +2011,10 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" t="s">
         <v>102</v>
-      </c>
-      <c r="C27" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2081,10 +2022,10 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>104</v>
+      </c>
+      <c r="C28" t="s">
         <v>106</v>
-      </c>
-      <c r="C28" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2092,10 +2033,10 @@
         <v>1</v>
       </c>
       <c r="B29" t="s">
+        <v>108</v>
+      </c>
+      <c r="C29" t="s">
         <v>110</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -2103,10 +2044,10 @@
         <v>1</v>
       </c>
       <c r="B30" t="s">
+        <v>112</v>
+      </c>
+      <c r="C30" t="s">
         <v>114</v>
-      </c>
-      <c r="C30" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -2114,10 +2055,10 @@
         <v>1</v>
       </c>
       <c r="B31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C31" t="s">
         <v>118</v>
-      </c>
-      <c r="C31" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -2125,32 +2066,32 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C32" t="s">
         <v>122</v>
-      </c>
-      <c r="C32" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" t="s">
+        <v>124</v>
+      </c>
+      <c r="C33" t="s">
         <v>126</v>
-      </c>
-      <c r="C33" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B34" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" t="s">
         <v>130</v>
-      </c>
-      <c r="C34" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -2158,10 +2099,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>132</v>
+      </c>
+      <c r="C35" t="s">
         <v>134</v>
-      </c>
-      <c r="C35" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2169,10 +2110,10 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C36" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -2180,10 +2121,10 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C37" t="s">
         <v>141</v>
-      </c>
-      <c r="C37" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -2191,10 +2132,10 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>143</v>
+      </c>
+      <c r="C38" t="s">
         <v>145</v>
-      </c>
-      <c r="C38" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -2202,10 +2143,10 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>147</v>
+      </c>
+      <c r="C39" t="s">
         <v>149</v>
-      </c>
-      <c r="C39" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -2213,10 +2154,10 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C40" t="s">
         <v>153</v>
-      </c>
-      <c r="C40" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -2224,10 +2165,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" t="s">
         <v>157</v>
-      </c>
-      <c r="C41" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2235,10 +2176,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -2246,10 +2187,10 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C43" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -2261,36 +2202,6 @@
       </c>
       <c r="C44" t="s">
         <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>177</v>
-      </c>
-      <c r="C47" t="s">
-        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
upsate to KiCad8, DNP 32KHz crystal, update BOM
</commit_message>
<xml_diff>
--- a/Manufacturing Files/bitaxeUltra BOM.xlsx
+++ b/Manufacturing Files/bitaxeUltra BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/skot/Work/Bitcoin/bitaxe/bitaxe-205/Manufacturing Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78B2B2FE-58A6-8D4F-9695-61E1868ABFF7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B4BECB-D6F6-1D4E-B6A9-867798663B3F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="500" windowWidth="28320" windowHeight="25240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="164">
   <si>
     <t>Qty</t>
   </si>
@@ -86,18 +86,6 @@
     <t>865080345012</t>
   </si>
   <si>
-    <t>C30, C31</t>
-  </si>
-  <si>
-    <t>6.8pF</t>
-  </si>
-  <si>
-    <t>399-C0402C689C5GAC7867CT-ND</t>
-  </si>
-  <si>
-    <t>C0402C689C5GAC7867</t>
-  </si>
-  <si>
     <t>C34, C36, C37</t>
   </si>
   <si>
@@ -522,18 +510,6 @@
   </si>
   <si>
     <t>BM1366_mode1</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>32.768kHz</t>
-  </si>
-  <si>
-    <t>728-1074-1-ND</t>
-  </si>
-  <si>
-    <t>SC32S-7PF20PPM</t>
   </si>
   <si>
     <t>NOPE</t>
@@ -927,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1026,7 +1002,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -1043,19 +1019,19 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>27</v>
-      </c>
-      <c r="E7" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -1063,10 +1039,10 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
@@ -1111,7 +1087,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -1128,7 +1104,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -1151,13 +1127,13 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" t="s">
         <v>49</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>50</v>
-      </c>
-      <c r="E13" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1165,10 +1141,10 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" t="s">
         <v>52</v>
-      </c>
-      <c r="C14" t="s">
-        <v>18</v>
       </c>
       <c r="D14" t="s">
         <v>53</v>
@@ -1191,7 +1167,7 @@
         <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1199,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>60</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>61</v>
-      </c>
-      <c r="E16" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1236,13 +1212,13 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" t="s">
         <v>67</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>68</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1250,10 +1226,10 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" t="s">
         <v>70</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
       </c>
       <c r="D19" t="s">
         <v>71</v>
@@ -1264,7 +1240,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -1276,29 +1252,29 @@
         <v>75</v>
       </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C21" t="s">
         <v>77</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>78</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>79</v>
-      </c>
-      <c r="E21" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>80</v>
@@ -1315,7 +1291,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>84</v>
@@ -1332,7 +1308,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -1349,7 +1325,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
@@ -1468,7 +1444,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>120</v>
@@ -1485,7 +1461,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
@@ -1514,7 +1490,7 @@
         <v>130</v>
       </c>
       <c r="E34" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1522,16 +1498,16 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
+        <v>131</v>
+      </c>
+      <c r="C35" t="s">
         <v>132</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>133</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>134</v>
-      </c>
-      <c r="E35" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
@@ -1616,7 +1592,7 @@
         <v>153</v>
       </c>
       <c r="E40" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1624,16 +1600,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
+        <v>154</v>
+      </c>
+      <c r="C41" t="s">
         <v>155</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>156</v>
       </c>
-      <c r="D41" t="s">
-        <v>157</v>
-      </c>
       <c r="E41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1641,16 +1617,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" t="s">
         <v>158</v>
       </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>159</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>160</v>
-      </c>
-      <c r="E42" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1665,40 +1641,6 @@
       </c>
       <c r="D43" t="s">
         <v>163</v>
-      </c>
-      <c r="E43" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>165</v>
-      </c>
-      <c r="C44" t="s">
-        <v>166</v>
-      </c>
-      <c r="D44" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>167</v>
-      </c>
-      <c r="C45" t="s">
-        <v>168</v>
-      </c>
-      <c r="D45" t="s">
-        <v>169</v>
-      </c>
-      <c r="E45" t="s">
-        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -1708,10 +1650,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D53" sqref="D53"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1777,7 +1719,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
@@ -1788,13 +1730,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B7" t="s">
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1802,7 +1744,7 @@
         <v>1</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -1832,7 +1774,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>40</v>
@@ -1843,7 +1785,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B12" t="s">
         <v>44</v>
@@ -1860,7 +1802,7 @@
         <v>48</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1868,7 +1810,7 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" t="s">
         <v>53</v>
@@ -1890,10 +1832,10 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1915,7 +1857,7 @@
         <v>66</v>
       </c>
       <c r="C18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1923,7 +1865,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
         <v>71</v>
@@ -1931,7 +1873,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B20" t="s">
         <v>73</v>
@@ -1942,18 +1884,18 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B22" t="s">
         <v>80</v>
@@ -1964,7 +1906,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
         <v>84</v>
@@ -1975,7 +1917,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" t="s">
         <v>88</v>
@@ -1986,7 +1928,7 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" t="s">
         <v>92</v>
@@ -2063,7 +2005,7 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" t="s">
         <v>120</v>
@@ -2074,7 +2016,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" t="s">
         <v>124</v>
@@ -2099,10 +2041,10 @@
         <v>1</v>
       </c>
       <c r="B35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -2165,10 +2107,10 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -2176,32 +2118,10 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>161</v>
-      </c>
-      <c r="C43" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>